<commit_message>
Reworked classes that operate with database. Added options for importing/exporting data into .npz file.
</commit_message>
<xml_diff>
--- a/xlsx/params.xlsx
+++ b/xlsx/params.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bandy\PycharmProjects\ElectricMotorCalc\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0A0EB47-5877-4EBB-9460-E14A018170E0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CE562D2-A4DF-4DD6-86A5-21A17B90E1F6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1515" yWindow="1515" windowWidth="21600" windowHeight="11835" xr2:uid="{DF5FBB1E-D8F3-401C-86E6-356286B5DD4B}"/>
   </bookViews>
@@ -629,7 +629,7 @@
   <dimension ref="A1:C40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -655,7 +655,7 @@
         <v>39</v>
       </c>
       <c r="B2" s="1">
-        <v>300</v>
+        <v>2</v>
       </c>
       <c r="C2" t="s">
         <v>0</v>
@@ -666,7 +666,7 @@
         <v>40</v>
       </c>
       <c r="B3" s="1">
-        <v>36</v>
+        <v>48</v>
       </c>
       <c r="C3" t="s">
         <v>1</v>

</xml_diff>